<commit_message>
account , logincenter , serverlist , createrole
</commit_message>
<xml_diff>
--- a/Excel/StartZoneConfig.xlsx
+++ b/Excel/StartZoneConfig.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20383"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\SourceCodes\ET\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_proj\ET-FrameAsync\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0266646D-12F4-4C45-ACA1-34E2C96C8F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7D64FA-A04B-4F69-80B0-AB91653ED15B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47325" yWindow="4395" windowWidth="25620" windowHeight="13260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,13 +43,15 @@
     <t>string</t>
   </si>
   <si>
-    <t>ET1</t>
-  </si>
-  <si>
-    <t>ET2</t>
-  </si>
-  <si>
     <t>mongodb://127.0.0.1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FA2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -444,7 +446,7 @@
   <dimension ref="C3:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -494,10 +496,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.3">
@@ -505,10 +507,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>